<commit_message>
Updates as per Udacity review feedback
</commit_message>
<xml_diff>
--- a/IncidentDuration_coef.xlsx
+++ b/IncidentDuration_coef.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>est_int</t>
   </si>
@@ -25,31 +25,13 @@
     <t>priority__Priority 4</t>
   </si>
   <si>
-    <t>appl_tier__Iron</t>
-  </si>
-  <si>
-    <t>contact_type__self-service</t>
-  </si>
-  <si>
-    <t>team__Specialist</t>
-  </si>
-  <si>
-    <t>contact_type__other</t>
+    <t>contact_type__Other</t>
   </si>
   <si>
     <t>inc_close_code__Information Provided / Training</t>
   </si>
   <si>
-    <t>contact_type__walk-in</t>
-  </si>
-  <si>
-    <t>contact_type__phone</t>
-  </si>
-  <si>
-    <t>inc_close_code__Data Correction</t>
-  </si>
-  <si>
-    <t>contact_type__chat</t>
+    <t>appl_tier__Silver</t>
   </si>
   <si>
     <t>inc_close_code__Software Correction</t>
@@ -58,22 +40,16 @@
     <t>inc_close_code__Environmental Restoration</t>
   </si>
   <si>
-    <t>appl_tier__Silver</t>
+    <t>inc_close_code__other</t>
   </si>
   <si>
     <t>inc_close_code__Security Modification</t>
   </si>
   <si>
-    <t>inc_close_code__other</t>
+    <t>appl_tier__Gold</t>
   </si>
   <si>
     <t>inc_close_code__Reboot / Restart</t>
-  </si>
-  <si>
-    <t>priority__other</t>
-  </si>
-  <si>
-    <t>appl_tier__Gold</t>
   </si>
 </sst>
 </file>
@@ -431,7 +407,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -447,68 +423,68 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2">
-        <v>1.603126135689519</v>
+        <v>1.347158825273615</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3">
-        <v>1.582030088410115</v>
+        <v>0.6454866656421309</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
-        <v>1.042071431017158</v>
+        <v>0.0589937550298763</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5">
-        <v>0.6995849453590227</v>
+        <v>-0.01820929942896091</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6">
-        <v>0.5133107257478144</v>
+        <v>-0.1462066704613506</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7">
-        <v>0.328494889741781</v>
+        <v>-0.2541199327167313</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -519,7 +495,7 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>0.2431662533879733</v>
+        <v>-0.3698442290367989</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -530,117 +506,29 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>0.2098949826736566</v>
+        <v>-0.5033290620130868</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
-        <v>0.1713590621275107</v>
+        <v>-0.8246668669285009</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11">
-        <v>0.1435562828894151</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12">
-        <v>0.07893911391661754</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13">
-        <v>0.07555385589139096</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1">
-        <v>2</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14">
-        <v>-0.01448430586054563</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15">
-        <v>-0.2267557504163897</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1">
-        <v>17</v>
-      </c>
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16">
-        <v>-0.2717905498314646</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1">
-        <v>14</v>
-      </c>
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17">
-        <v>-0.6753869596215253</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18">
-        <v>-0.7136250178133361</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1">
-        <v>0</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19">
-        <v>-0.857691345998724</v>
+        <v>-0.9915309789430951</v>
       </c>
     </row>
   </sheetData>

</xml_diff>